<commit_message>
testing 3er grupo de excel
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_003_ConstanciasFiscalesBancoTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_003_ConstanciasFiscalesBancoTest.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A23E44-50AB-41D1-854F-8981AD8613B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AA3F5B-DE0C-48FD-AB11-F5CF7F94A023}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Escenario</t>
   </si>
@@ -37,15 +37,6 @@
     <t>Paso3</t>
   </si>
   <si>
-    <t>TC_003_01_agregarProducto</t>
-  </si>
-  <si>
-    <t>Navegamos a la página principal y entramos a la sección de ratones.||Paso realizado correctamente.</t>
-  </si>
-  <si>
-    <t>Elegimos un ratón y clickeamos en él.||Click realizado correctamente.</t>
-  </si>
-  <si>
     <t>Paso4</t>
   </si>
   <si>
@@ -58,28 +49,34 @@
     <t>Paso7</t>
   </si>
   <si>
-    <t>Navegamos a la página del producto y lo añadimos al carrito.||Click al botón addToCart realizado.</t>
-  </si>
-  <si>
-    <t>El ratón se añadió correctamente||Producto añadido correctamente.</t>
-  </si>
-  <si>
-    <t>TC_003_02_usuarioExistente</t>
-  </si>
-  <si>
-    <t>Navegamos a la página principal y clickeamos en el botón User.||Click realizado correctamente.</t>
-  </si>
-  <si>
-    <t>Se abre un popup y clickeamos en el Link CreateNewAccount||Click realizado correctamente</t>
-  </si>
-  <si>
-    <t>Rellenamos los campos del formulario.||Campos completados.</t>
-  </si>
-  <si>
-    <t>Aceptamos las condiciones y clickeamos en crear cuenta.||Pasos realizados correctamente.</t>
-  </si>
-  <si>
-    <t>Se muestra el mensaje de que ya existe el usuario que intentamos crear.||User name already exists.</t>
+    <t>SC_003_01_ConsultaYDescargaClienteBancoIngles</t>
+  </si>
+  <si>
+    <t>Navegamos a la página principal y entramos en el home page.||Paso realizado correctamente.</t>
+  </si>
+  <si>
+    <t>Seleccionar idioma Inglés y  la opción de "Idioma" .||Click realizado correctamente.</t>
+  </si>
+  <si>
+    <t>Seleccionar el Rol Bank Client||Click al botón Bank Client.</t>
+  </si>
+  <si>
+    <t>Rellenamos los campos de datos, aceptamos condiciones y presionamos el botón Ok||Pasos realizados correctamente.</t>
+  </si>
+  <si>
+    <t>Seleccionamos el Año Fiscal  y presionar el botón Consultar||Pasos realizados correctamente.</t>
+  </si>
+  <si>
+    <t>En la columna Type of request le damos click al icono de DOWNLOAD para descargar la constancia||Click realizado correctamente.</t>
+  </si>
+  <si>
+    <t>SC_003_02_ConsultaYDescargaClienteBancoEspañol</t>
+  </si>
+  <si>
+    <t>Seleccionar el Rol Cliente banco||Click al botón Cliente banco.</t>
+  </si>
+  <si>
+    <t>Seleccionar idioma Español y la opción de "Idioma" .||Click realizado correctamente.</t>
   </si>
 </sst>
 </file>
@@ -414,19 +411,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -446,28 +444,28 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
@@ -475,26 +473,35 @@
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se sube actualización y finalización de los escenarios de "Constancias Fiscales Banco"
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_003_ConstanciasFiscalesBancoTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_003_ConstanciasFiscalesBancoTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AA3F5B-DE0C-48FD-AB11-F5CF7F94A023}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3F1C64-81B6-413E-95B5-007FEAB86740}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="51">
   <si>
     <t>Escenario</t>
   </si>
@@ -52,12 +52,6 @@
     <t>SC_003_01_ConsultaYDescargaClienteBancoIngles</t>
   </si>
   <si>
-    <t>Navegamos a la página principal y entramos en el home page.||Paso realizado correctamente.</t>
-  </si>
-  <si>
-    <t>Seleccionar idioma Inglés y  la opción de "Idioma" .||Click realizado correctamente.</t>
-  </si>
-  <si>
     <t>Seleccionar el Rol Bank Client||Click al botón Bank Client.</t>
   </si>
   <si>
@@ -76,7 +70,109 @@
     <t>Seleccionar el Rol Cliente banco||Click al botón Cliente banco.</t>
   </si>
   <si>
-    <t>Seleccionar idioma Español y la opción de "Idioma" .||Click realizado correctamente.</t>
+    <t>SC_003_03_ConsultayDescargaClienteCasaDeBolsaIngles</t>
+  </si>
+  <si>
+    <t>SC_003_04_ConsultayDescargaClienteCasaDeBolsaEspañol</t>
+  </si>
+  <si>
+    <t>SC_003_05_ConsultayDescargaClienteMexderIngles</t>
+  </si>
+  <si>
+    <t>SC_003_06_ConsultayDescargaClienteMexderEspañol</t>
+  </si>
+  <si>
+    <t>SC_003_07_ConsultaYDescargaClienteOTCIngles</t>
+  </si>
+  <si>
+    <t>SC_003_08_ConsultayDescargaOTCEspañol</t>
+  </si>
+  <si>
+    <t>SC_003_09_ConsultaYDescargaProveedorInglesExtranjero</t>
+  </si>
+  <si>
+    <t>SC_003_10_ConsultaYDescargaProveedorEspañolExtranjero</t>
+  </si>
+  <si>
+    <t>SC_003_11_ConsultaYDescargaPremiadoIngles</t>
+  </si>
+  <si>
+    <t>SC_003_12_ConsultaYDescargaPremiadoEspañol</t>
+  </si>
+  <si>
+    <t>SC_003_13_ConsultaYDescargaClienteBancoIngles</t>
+  </si>
+  <si>
+    <t>SC_003_14_ConsultaYDescargaClienteBancoEspañol</t>
+  </si>
+  <si>
+    <t>SC_003_15_ConsultaYDescargaClienteCasaDeBolsaIngles</t>
+  </si>
+  <si>
+    <t>SC_003_16_ConsultaYDescargaClienteCasaDeBolsaEspañol</t>
+  </si>
+  <si>
+    <t>SC_003_17_ConsultaYDescargaClienteMexderIngles</t>
+  </si>
+  <si>
+    <t>SC_003_18_ConsultaYDescargaClienteMexderEspañol</t>
+  </si>
+  <si>
+    <t>SC_003_19_ConsultaYDescargaClienteOTCIngles</t>
+  </si>
+  <si>
+    <t>SC_003_20_ConsultaYDescargaOTCEspañol</t>
+  </si>
+  <si>
+    <t>SC_003_21_ConsultaYDescargaProveedorInglesExtranjero</t>
+  </si>
+  <si>
+    <t>SC_003_22_ConsultaYDescargaProveedorEspañolExtranjero</t>
+  </si>
+  <si>
+    <t>SC_003_23_ConsultaYDescargaPremiadoIngles</t>
+  </si>
+  <si>
+    <t>SC_003_24_ConsultaYDescargaPremiadoEspañol</t>
+  </si>
+  <si>
+    <t>Seleccionar idioma Inglés y  del menú de "Idioma"||Click realizado correctamente.</t>
+  </si>
+  <si>
+    <t>Navegamos a la página principal y entramos en el home page||Paso realizado correctamente.</t>
+  </si>
+  <si>
+    <t>Seleccionar idioma Español y  del menú de "Idioma"||Click realizado correctamente.</t>
+  </si>
+  <si>
+    <t>Validamos que se descargue el pdf correspondiente al cliente y el año fiscal||El documento se descargo correctamente</t>
+  </si>
+  <si>
+    <t>Seleccionar el Rol Cliente Casa de Bolsa||Click al botón Cliente banco.</t>
+  </si>
+  <si>
+    <t>Seleccionar el Rol MexDer||Click al botón Cliente banco.</t>
+  </si>
+  <si>
+    <t>Seleccionar el Rol Proveedor||Click al botón Cliente banco.</t>
+  </si>
+  <si>
+    <t>Seleccionar el Rol Premiado||Click al botón Cliente banco.</t>
+  </si>
+  <si>
+    <t>Seleccionar el Rol Bank Client||Click al botón Cliente banco.</t>
+  </si>
+  <si>
+    <t>Seleccionar el RolMexDer||Click al botón Cliente banco.</t>
+  </si>
+  <si>
+    <t>Seleccionar el RolProveedor||Click al botón Cliente banco.</t>
+  </si>
+  <si>
+    <t>Seleccionamos la opción Proveedor Extranjero||Click realizado exitosamente.</t>
+  </si>
+  <si>
+    <t>Paso8</t>
   </si>
 </sst>
 </file>
@@ -409,25 +505,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,156 +553,676 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>